<commit_message>
update urban_ath non_rep, trimester and yearly
</commit_message>
<xml_diff>
--- a/dictionaries/urban_ath/1_0/1_0_non_rep.xlsx
+++ b/dictionaries/urban_ath/1_0/1_0_non_rep.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26412"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26415"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="3" documentId="11_AF755BB544E45B5F7270BD190789DF5784D64760" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A3DFD2D4-05DD-40E7-9D48-9AC994960BAE}"/>
+  <xr:revisionPtr revIDLastSave="7" documentId="11_AF755BB544E45B5F7270BD190789DF5784D64760" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9F81EF70-9D14-4ED8-B743-271D6A502AAB}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -93,7 +93,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="892" uniqueCount="454">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="894" uniqueCount="455">
   <si>
     <t>name</t>
   </si>
@@ -1304,10 +1304,13 @@
     <t>hgs</t>
   </si>
   <si>
-    <t>recetox</t>
+    <t>elspac</t>
   </si>
   <si>
     <t>genxxi</t>
+  </si>
+  <si>
+    <t>genrnext</t>
   </si>
   <si>
     <t>city</t>
@@ -4645,10 +4648,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:D109"/>
+  <dimension ref="A1:D110"/>
   <sheetViews>
     <sheetView showFormulas="1" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C105" sqref="C105"/>
+      <selection activeCell="A33" sqref="A33:XFD33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="12.75"/>
@@ -5107,12 +5110,12 @@
     </row>
     <row r="33" spans="1:4">
       <c r="A33" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B33">
-        <v>30</v>
-      </c>
-      <c r="C33" t="b">
+        <v>132</v>
+      </c>
+      <c r="C33" s="1" t="b">
         <v>0</v>
       </c>
       <c r="D33" t="s">
@@ -5124,7 +5127,7 @@
         <v>13</v>
       </c>
       <c r="B34">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="C34" t="b">
         <v>0</v>
@@ -5138,7 +5141,7 @@
         <v>13</v>
       </c>
       <c r="B35">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C35" t="b">
         <v>0</v>
@@ -5152,7 +5155,7 @@
         <v>13</v>
       </c>
       <c r="B36">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C36" t="b">
         <v>0</v>
@@ -5166,7 +5169,7 @@
         <v>13</v>
       </c>
       <c r="B37">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="C37" t="b">
         <v>0</v>
@@ -5180,7 +5183,7 @@
         <v>13</v>
       </c>
       <c r="B38">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C38" t="b">
         <v>0</v>
@@ -5194,7 +5197,7 @@
         <v>13</v>
       </c>
       <c r="B39">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C39" t="b">
         <v>0</v>
@@ -5208,7 +5211,7 @@
         <v>13</v>
       </c>
       <c r="B40">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C40" t="b">
         <v>0</v>
@@ -5219,10 +5222,10 @@
     </row>
     <row r="41" spans="1:4">
       <c r="A41" t="s">
-        <v>231</v>
+        <v>13</v>
       </c>
       <c r="B41">
-        <v>1001</v>
+        <v>10</v>
       </c>
       <c r="C41" t="b">
         <v>0</v>
@@ -5236,7 +5239,7 @@
         <v>231</v>
       </c>
       <c r="B42">
-        <v>1102</v>
+        <v>1001</v>
       </c>
       <c r="C42" t="b">
         <v>0</v>
@@ -5250,7 +5253,7 @@
         <v>231</v>
       </c>
       <c r="B43">
-        <v>1103</v>
+        <v>1102</v>
       </c>
       <c r="C43" t="b">
         <v>0</v>
@@ -5264,7 +5267,7 @@
         <v>231</v>
       </c>
       <c r="B44">
-        <v>1104</v>
+        <v>1103</v>
       </c>
       <c r="C44" t="b">
         <v>0</v>
@@ -5278,7 +5281,7 @@
         <v>231</v>
       </c>
       <c r="B45">
-        <v>1201</v>
+        <v>1104</v>
       </c>
       <c r="C45" t="b">
         <v>0</v>
@@ -5292,7 +5295,7 @@
         <v>231</v>
       </c>
       <c r="B46">
-        <v>1202</v>
+        <v>1201</v>
       </c>
       <c r="C46" t="b">
         <v>0</v>
@@ -5306,7 +5309,7 @@
         <v>231</v>
       </c>
       <c r="B47">
-        <v>1203</v>
+        <v>1202</v>
       </c>
       <c r="C47" t="b">
         <v>0</v>
@@ -5320,7 +5323,7 @@
         <v>231</v>
       </c>
       <c r="B48">
-        <v>1204</v>
+        <v>1203</v>
       </c>
       <c r="C48" t="b">
         <v>0</v>
@@ -5334,7 +5337,7 @@
         <v>231</v>
       </c>
       <c r="B49">
-        <v>1205</v>
+        <v>1204</v>
       </c>
       <c r="C49" t="b">
         <v>0</v>
@@ -5348,7 +5351,7 @@
         <v>231</v>
       </c>
       <c r="B50">
-        <v>1301</v>
+        <v>1205</v>
       </c>
       <c r="C50" t="b">
         <v>0</v>
@@ -5362,7 +5365,7 @@
         <v>231</v>
       </c>
       <c r="B51">
-        <v>1401</v>
+        <v>1301</v>
       </c>
       <c r="C51" t="b">
         <v>0</v>
@@ -5376,7 +5379,7 @@
         <v>231</v>
       </c>
       <c r="B52">
-        <v>1402</v>
+        <v>1401</v>
       </c>
       <c r="C52" t="b">
         <v>0</v>
@@ -5390,7 +5393,7 @@
         <v>231</v>
       </c>
       <c r="B53">
-        <v>1403</v>
+        <v>1402</v>
       </c>
       <c r="C53" t="b">
         <v>0</v>
@@ -5404,7 +5407,7 @@
         <v>231</v>
       </c>
       <c r="B54">
-        <v>1404</v>
+        <v>1403</v>
       </c>
       <c r="C54" t="b">
         <v>0</v>
@@ -5418,7 +5421,7 @@
         <v>231</v>
       </c>
       <c r="B55">
-        <v>1501</v>
+        <v>1404</v>
       </c>
       <c r="C55" t="b">
         <v>0</v>
@@ -5432,7 +5435,7 @@
         <v>231</v>
       </c>
       <c r="B56">
-        <v>1601</v>
+        <v>1501</v>
       </c>
       <c r="C56" t="b">
         <v>0</v>
@@ -5446,7 +5449,7 @@
         <v>231</v>
       </c>
       <c r="B57">
-        <v>1701</v>
+        <v>1601</v>
       </c>
       <c r="C57" t="b">
         <v>0</v>
@@ -5460,7 +5463,7 @@
         <v>231</v>
       </c>
       <c r="B58">
-        <v>1801</v>
+        <v>1701</v>
       </c>
       <c r="C58" t="b">
         <v>0</v>
@@ -5474,7 +5477,7 @@
         <v>231</v>
       </c>
       <c r="B59">
-        <v>1802</v>
+        <v>1801</v>
       </c>
       <c r="C59" t="b">
         <v>0</v>
@@ -5488,7 +5491,7 @@
         <v>231</v>
       </c>
       <c r="B60">
-        <v>1803</v>
+        <v>1802</v>
       </c>
       <c r="C60" t="b">
         <v>0</v>
@@ -5502,7 +5505,7 @@
         <v>231</v>
       </c>
       <c r="B61">
-        <v>1901</v>
+        <v>1803</v>
       </c>
       <c r="C61" t="b">
         <v>0</v>
@@ -5516,7 +5519,7 @@
         <v>231</v>
       </c>
       <c r="B62">
-        <v>1803</v>
+        <v>1901</v>
       </c>
       <c r="C62" t="b">
         <v>0</v>
@@ -5530,7 +5533,7 @@
         <v>231</v>
       </c>
       <c r="B63">
-        <v>2101</v>
+        <v>1804</v>
       </c>
       <c r="C63" t="b">
         <v>0</v>
@@ -5544,7 +5547,7 @@
         <v>231</v>
       </c>
       <c r="B64">
-        <v>2201</v>
+        <v>2101</v>
       </c>
       <c r="C64" t="b">
         <v>0</v>
@@ -5558,7 +5561,7 @@
         <v>231</v>
       </c>
       <c r="B65">
-        <v>2301</v>
+        <v>2201</v>
       </c>
       <c r="C65" t="b">
         <v>0</v>
@@ -5569,10 +5572,10 @@
     </row>
     <row r="66" spans="1:4">
       <c r="A66" t="s">
-        <v>25</v>
+        <v>231</v>
       </c>
       <c r="B66">
-        <v>1</v>
+        <v>2301</v>
       </c>
       <c r="C66" t="b">
         <v>0</v>
@@ -5586,7 +5589,7 @@
         <v>25</v>
       </c>
       <c r="B67">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C67" t="b">
         <v>0</v>
@@ -5600,7 +5603,7 @@
         <v>25</v>
       </c>
       <c r="B68">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C68" t="b">
         <v>0</v>
@@ -5611,16 +5614,16 @@
     </row>
     <row r="69" spans="1:4">
       <c r="A69" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B69">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C69" t="b">
         <v>0</v>
       </c>
       <c r="D69" t="s">
-        <v>438</v>
+        <v>441</v>
       </c>
     </row>
     <row r="70" spans="1:4">
@@ -5628,13 +5631,13 @@
         <v>23</v>
       </c>
       <c r="B70">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C70" t="b">
         <v>0</v>
       </c>
       <c r="D70" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
     </row>
     <row r="71" spans="1:4">
@@ -5642,13 +5645,13 @@
         <v>23</v>
       </c>
       <c r="B71">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C71" t="b">
         <v>0</v>
       </c>
       <c r="D71" t="s">
-        <v>439</v>
+        <v>442</v>
       </c>
     </row>
     <row r="72" spans="1:4">
@@ -5656,13 +5659,13 @@
         <v>23</v>
       </c>
       <c r="B72">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C72" t="b">
         <v>0</v>
       </c>
       <c r="D72" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
     </row>
     <row r="73" spans="1:4">
@@ -5670,27 +5673,27 @@
         <v>23</v>
       </c>
       <c r="B73">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C73" t="b">
         <v>0</v>
       </c>
       <c r="D73" t="s">
-        <v>440</v>
+        <v>443</v>
       </c>
     </row>
     <row r="74" spans="1:4">
       <c r="A74" t="s">
-        <v>75</v>
+        <v>23</v>
       </c>
       <c r="B74">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C74" t="b">
         <v>0</v>
       </c>
       <c r="D74" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
     </row>
     <row r="75" spans="1:4">
@@ -5698,7 +5701,7 @@
         <v>75</v>
       </c>
       <c r="B75">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C75" t="b">
         <v>0</v>
@@ -5712,7 +5715,7 @@
         <v>75</v>
       </c>
       <c r="B76">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C76" t="b">
         <v>0</v>
@@ -5726,7 +5729,7 @@
         <v>75</v>
       </c>
       <c r="B77">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C77" t="b">
         <v>0</v>
@@ -5740,7 +5743,7 @@
         <v>75</v>
       </c>
       <c r="B78">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C78" t="b">
         <v>0</v>
@@ -5754,7 +5757,7 @@
         <v>75</v>
       </c>
       <c r="B79">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C79" t="b">
         <v>0</v>
@@ -5765,10 +5768,10 @@
     </row>
     <row r="80" spans="1:4">
       <c r="A80" t="s">
-        <v>89</v>
+        <v>75</v>
       </c>
       <c r="B80">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C80" t="b">
         <v>0</v>
@@ -5782,7 +5785,7 @@
         <v>89</v>
       </c>
       <c r="B81">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C81" t="b">
         <v>0</v>
@@ -5796,13 +5799,13 @@
         <v>89</v>
       </c>
       <c r="B82">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C82" t="b">
         <v>0</v>
       </c>
       <c r="D82" t="s">
-        <v>444</v>
+        <v>451</v>
       </c>
     </row>
     <row r="83" spans="1:4">
@@ -5810,7 +5813,7 @@
         <v>89</v>
       </c>
       <c r="B83">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C83" t="b">
         <v>0</v>
@@ -5824,7 +5827,7 @@
         <v>89</v>
       </c>
       <c r="B84">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C84" t="b">
         <v>0</v>
@@ -5838,21 +5841,21 @@
         <v>89</v>
       </c>
       <c r="B85">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C85" t="b">
         <v>0</v>
       </c>
       <c r="D85" t="s">
-        <v>451</v>
+        <v>447</v>
       </c>
     </row>
     <row r="86" spans="1:4">
       <c r="A86" t="s">
-        <v>38</v>
+        <v>89</v>
       </c>
       <c r="B86">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="C86" t="b">
         <v>0</v>
@@ -5863,10 +5866,10 @@
     </row>
     <row r="87" spans="1:4">
       <c r="A87" t="s">
-        <v>59</v>
+        <v>38</v>
       </c>
       <c r="B87">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C87" t="b">
         <v>0</v>
@@ -5877,7 +5880,7 @@
     </row>
     <row r="88" spans="1:4">
       <c r="A88" t="s">
-        <v>239</v>
+        <v>59</v>
       </c>
       <c r="B88">
         <v>1</v>
@@ -5886,7 +5889,7 @@
         <v>0</v>
       </c>
       <c r="D88" t="s">
-        <v>438</v>
+        <v>454</v>
       </c>
     </row>
     <row r="89" spans="1:4">
@@ -5894,7 +5897,7 @@
         <v>239</v>
       </c>
       <c r="B89">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C89" t="b">
         <v>0</v>
@@ -5908,7 +5911,7 @@
         <v>239</v>
       </c>
       <c r="B90">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C90" t="b">
         <v>0</v>
@@ -5919,16 +5922,16 @@
     </row>
     <row r="91" spans="1:4">
       <c r="A91" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="B91">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C91" t="b">
         <v>0</v>
       </c>
       <c r="D91" t="s">
-        <v>438</v>
+        <v>441</v>
       </c>
     </row>
     <row r="92" spans="1:4">
@@ -5936,13 +5939,13 @@
         <v>237</v>
       </c>
       <c r="B92">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C92" t="b">
         <v>0</v>
       </c>
       <c r="D92" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
     </row>
     <row r="93" spans="1:4">
@@ -5950,13 +5953,13 @@
         <v>237</v>
       </c>
       <c r="B93">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C93" t="b">
         <v>0</v>
       </c>
       <c r="D93" t="s">
-        <v>439</v>
+        <v>442</v>
       </c>
     </row>
     <row r="94" spans="1:4">
@@ -5964,13 +5967,13 @@
         <v>237</v>
       </c>
       <c r="B94">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C94" t="b">
         <v>0</v>
       </c>
       <c r="D94" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
     </row>
     <row r="95" spans="1:4">
@@ -5978,27 +5981,27 @@
         <v>237</v>
       </c>
       <c r="B95">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C95" t="b">
         <v>0</v>
       </c>
       <c r="D95" t="s">
-        <v>440</v>
+        <v>443</v>
       </c>
     </row>
     <row r="96" spans="1:4">
       <c r="A96" t="s">
-        <v>275</v>
+        <v>237</v>
       </c>
       <c r="B96">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C96" t="b">
         <v>0</v>
       </c>
       <c r="D96" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
     </row>
     <row r="97" spans="1:4">
@@ -6006,7 +6009,7 @@
         <v>275</v>
       </c>
       <c r="B97">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C97" t="b">
         <v>0</v>
@@ -6020,7 +6023,7 @@
         <v>275</v>
       </c>
       <c r="B98">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C98" t="b">
         <v>0</v>
@@ -6034,7 +6037,7 @@
         <v>275</v>
       </c>
       <c r="B99">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C99" t="b">
         <v>0</v>
@@ -6048,7 +6051,7 @@
         <v>275</v>
       </c>
       <c r="B100">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C100" t="b">
         <v>0</v>
@@ -6062,7 +6065,7 @@
         <v>275</v>
       </c>
       <c r="B101">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C101" t="b">
         <v>0</v>
@@ -6073,10 +6076,10 @@
     </row>
     <row r="102" spans="1:4">
       <c r="A102" t="s">
-        <v>287</v>
+        <v>275</v>
       </c>
       <c r="B102">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C102" t="b">
         <v>0</v>
@@ -6090,7 +6093,7 @@
         <v>287</v>
       </c>
       <c r="B103">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C103" t="b">
         <v>0</v>
@@ -6104,13 +6107,13 @@
         <v>287</v>
       </c>
       <c r="B104">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C104" t="b">
         <v>0</v>
       </c>
       <c r="D104" t="s">
-        <v>444</v>
+        <v>451</v>
       </c>
     </row>
     <row r="105" spans="1:4">
@@ -6118,7 +6121,7 @@
         <v>287</v>
       </c>
       <c r="B105">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C105" t="b">
         <v>0</v>
@@ -6132,7 +6135,7 @@
         <v>287</v>
       </c>
       <c r="B106">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C106" t="b">
         <v>0</v>
@@ -6146,21 +6149,21 @@
         <v>287</v>
       </c>
       <c r="B107">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C107" t="b">
         <v>0</v>
       </c>
       <c r="D107" t="s">
-        <v>451</v>
+        <v>447</v>
       </c>
     </row>
     <row r="108" spans="1:4">
       <c r="A108" t="s">
-        <v>249</v>
+        <v>287</v>
       </c>
       <c r="B108">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="C108" t="b">
         <v>0</v>
@@ -6171,16 +6174,30 @@
     </row>
     <row r="109" spans="1:4">
       <c r="A109" t="s">
-        <v>267</v>
+        <v>249</v>
       </c>
       <c r="B109">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C109" t="b">
         <v>0</v>
       </c>
       <c r="D109" t="s">
         <v>453</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4">
+      <c r="A110" t="s">
+        <v>267</v>
+      </c>
+      <c r="B110">
+        <v>1</v>
+      </c>
+      <c r="C110" t="b">
+        <v>0</v>
+      </c>
+      <c r="D110" t="s">
+        <v>454</v>
       </c>
     </row>
   </sheetData>

</xml_diff>